<commit_message>
Implemented fake data to post on mqtt topics
</commit_message>
<xml_diff>
--- a/AQI_Breakingpoints.xlsx
+++ b/AQI_Breakingpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netcompany-my.sharepoint.com/personal/ckiokak_netcompany_com/Documents/Documents/IoT/IoT-APARS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFB4ED94-A02A-4AB9-BF66-26D3E41130D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{EFB4ED94-A02A-4AB9-BF66-26D3E41130D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88CC3507-B70A-41D3-ABE4-7B3AB7DA1B36}"/>
   <bookViews>
-    <workbookView xWindow="-4635" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{692AA805-449B-43EB-A383-3CF970FA8A04}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{692AA805-449B-43EB-A383-3CF970FA8A04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +142,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7C53CD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -210,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -218,10 +260,31 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -230,6 +293,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF7C53CD"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -560,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EBFE2D9-CA93-4289-B30C-E10B9B3ADE67}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -575,7 +643,7 @@
     <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -605,7 +673,7 @@
       <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="3">
@@ -628,7 +696,7 @@
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="3">
@@ -674,7 +742,7 @@
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="3">
@@ -697,7 +765,7 @@
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="3">
@@ -720,7 +788,7 @@
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="3">
@@ -737,140 +805,140 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="5">
         <v>0</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="5">
         <v>50</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="5">
         <v>0</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="6">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="5">
         <v>51</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="5">
         <v>100</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="5">
         <v>9.1</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="6">
         <v>35.4</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="5">
         <v>101</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="5">
         <v>150</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="5">
         <v>35.5</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="6">
         <v>55.4</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="5">
         <v>151</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="5">
         <v>200</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="5">
         <v>55.5</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="6">
         <v>125.4</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="5">
         <v>201</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="5">
         <v>300</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="5">
         <v>125.5</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="6">
         <v>225.4</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="5">
         <v>301</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="5">
         <v>500</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="5">
         <v>225.5</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="6">
         <v>500</v>
       </c>
     </row>
@@ -881,7 +949,7 @@
       <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="3">
@@ -893,7 +961,7 @@
       <c r="F14" s="3">
         <v>0</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>54</v>
       </c>
     </row>
@@ -904,7 +972,7 @@
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="3">
@@ -916,7 +984,7 @@
       <c r="F15" s="3">
         <v>54.1</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>154</v>
       </c>
     </row>
@@ -939,7 +1007,7 @@
       <c r="F16" s="3">
         <v>154.1</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <v>254</v>
       </c>
     </row>
@@ -950,7 +1018,7 @@
       <c r="B17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="3">
@@ -962,7 +1030,7 @@
       <c r="F17" s="3">
         <v>254.1</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>354</v>
       </c>
     </row>
@@ -973,7 +1041,7 @@
       <c r="B18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="3">
@@ -985,7 +1053,7 @@
       <c r="F18" s="3">
         <v>354.1</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>424</v>
       </c>
     </row>
@@ -996,7 +1064,7 @@
       <c r="B19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="3">
@@ -1008,145 +1076,145 @@
       <c r="F19" s="3">
         <v>424.1</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>604</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="B20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="5">
         <v>0</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="5">
         <v>50</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="5">
         <v>0</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="5">
         <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="B21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="5">
         <v>51</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="5">
         <v>100</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="5">
         <v>200.1</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="5">
         <v>400</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="5">
         <v>101</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="5">
         <v>150</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="5">
         <v>400.1</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="5">
         <v>800</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="B23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="5">
         <v>151</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="5">
         <v>200</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="5">
         <v>800.1</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="5">
         <v>1200</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="5">
         <v>201</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="5">
         <v>300</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="5">
         <v>1200.0999999999999</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="5">
         <v>1800</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="B25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="5">
         <v>301</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="5">
         <v>500</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="5">
         <v>1800.1</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="5">
         <v>2400</v>
       </c>
     </row>
@@ -1157,7 +1225,7 @@
       <c r="B26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D26" s="3">
@@ -1169,7 +1237,7 @@
       <c r="F26" s="3">
         <v>0</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="3">
         <v>100</v>
       </c>
     </row>
@@ -1180,7 +1248,7 @@
       <c r="B27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="3">
@@ -1192,7 +1260,7 @@
       <c r="F27" s="3">
         <v>100.1</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="3">
         <v>200</v>
       </c>
     </row>
@@ -1215,7 +1283,7 @@
       <c r="F28" s="3">
         <v>200.1</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="3">
         <v>300</v>
       </c>
     </row>
@@ -1226,7 +1294,7 @@
       <c r="B29" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="3">
@@ -1238,7 +1306,7 @@
       <c r="F29" s="3">
         <v>300.10000000000002</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="3">
         <v>400</v>
       </c>
     </row>
@@ -1249,7 +1317,7 @@
       <c r="B30" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D30" s="3">
@@ -1261,7 +1329,7 @@
       <c r="F30" s="3">
         <v>400.1</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="3">
         <v>500</v>
       </c>
     </row>
@@ -1272,7 +1340,7 @@
       <c r="B31" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="3">
@@ -1284,145 +1352,145 @@
       <c r="F31" s="3">
         <v>500.1</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="3">
         <v>600</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="B32" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="5">
         <v>0</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="5">
         <v>50</v>
       </c>
-      <c r="F32" s="3">
+      <c r="F32" s="5">
         <v>0</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32" s="5">
         <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="B33" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="5">
         <v>51</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="5">
         <v>100</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="5">
         <v>100.1</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="5">
         <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="B34" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="5">
         <v>101</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="5">
         <v>150</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="5">
         <v>200.1</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="5">
         <v>300</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" s="3" t="s">
+      <c r="B35" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="5">
         <v>151</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="5">
         <v>200</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="5">
         <v>300.10000000000002</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="5">
         <v>400</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="B36" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="5">
         <v>201</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="5">
         <v>300</v>
       </c>
-      <c r="F36" s="3">
+      <c r="F36" s="5">
         <v>400.1</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="5">
         <v>500</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="3" t="s">
+      <c r="B37" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="5">
         <v>301</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="5">
         <v>500</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F37" s="5">
         <v>500.1</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37" s="5">
         <v>600</v>
       </c>
     </row>
@@ -1433,7 +1501,7 @@
       <c r="B38" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D38" s="3">
@@ -1445,7 +1513,7 @@
       <c r="F38" s="3">
         <v>0</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38" s="3">
         <v>350</v>
       </c>
     </row>
@@ -1456,7 +1524,7 @@
       <c r="B39" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D39" s="3">
@@ -1468,7 +1536,7 @@
       <c r="F39" s="3">
         <v>350.1</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="3">
         <v>600</v>
       </c>
     </row>
@@ -1491,7 +1559,7 @@
       <c r="F40" s="3">
         <v>600.1</v>
       </c>
-      <c r="G40" s="4">
+      <c r="G40" s="3">
         <v>1000</v>
       </c>
     </row>
@@ -1502,7 +1570,7 @@
       <c r="B41" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D41" s="3">
@@ -1514,7 +1582,7 @@
       <c r="F41" s="3">
         <v>1000.1</v>
       </c>
-      <c r="G41" s="4">
+      <c r="G41" s="3">
         <v>1500</v>
       </c>
     </row>
@@ -1525,7 +1593,7 @@
       <c r="B42" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="3">
@@ -1537,7 +1605,7 @@
       <c r="F42" s="3">
         <v>1500.1</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G42" s="3">
         <v>2000</v>
       </c>
     </row>
@@ -1548,7 +1616,7 @@
       <c r="B43" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D43" s="3">
@@ -1560,145 +1628,145 @@
       <c r="F43" s="3">
         <v>2000.1</v>
       </c>
-      <c r="G43" s="4">
+      <c r="G43" s="3">
         <v>5000</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" s="3" t="s">
+      <c r="B44" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="5">
         <v>0</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="5">
         <v>50</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44" s="5">
         <v>0</v>
       </c>
-      <c r="G44" s="4">
+      <c r="G44" s="5">
         <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" s="3" t="s">
+      <c r="B45" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="5">
         <v>51</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="5">
         <v>100</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45" s="5">
         <v>54.1</v>
       </c>
-      <c r="G45" s="4">
+      <c r="G45" s="5">
         <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" s="3" t="s">
+      <c r="B46" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="5">
         <v>101</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="5">
         <v>150</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F46" s="5">
         <v>154.1</v>
       </c>
-      <c r="G46" s="4">
+      <c r="G46" s="5">
         <v>254</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" s="3" t="s">
+      <c r="B47" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="5">
         <v>151</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="5">
         <v>200</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F47" s="5">
         <v>254.1</v>
       </c>
-      <c r="G47" s="4">
+      <c r="G47" s="5">
         <v>354</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" s="3" t="s">
+      <c r="B48" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="5">
         <v>201</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="5">
         <v>300</v>
       </c>
-      <c r="F48" s="3">
+      <c r="F48" s="5">
         <v>354.1</v>
       </c>
-      <c r="G48" s="4">
+      <c r="G48" s="5">
         <v>424</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C49" s="3" t="s">
+      <c r="B49" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="5">
         <v>301</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="5">
         <v>500</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F49" s="5">
         <v>424.1</v>
       </c>
-      <c r="G49" s="4">
+      <c r="G49" s="5">
         <v>604</v>
       </c>
     </row>

</xml_diff>